<commit_message>
Added POM support to parser and added read POM commands.
More cleanup...
</commit_message>
<xml_diff>
--- a/src/CommInterface/DCCEX-commands.xlsx
+++ b/src/CommInterface/DCCEX-commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davidcutting42\src\CommandStation-DCC\.pio\libdeps\samd21\CommandStation\src\CommInterface\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{443F5A42-C8F4-41B5-9130-B59519B4940A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128305C1-9278-467E-BF20-D32E87FC58FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{03B09B78-E6DF-4BC3-A68B-D67D20DF6376}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="129">
   <si>
     <t>Param 1</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>payload (HEX)</t>
+  </si>
+  <si>
+    <t>Read CV byte on main</t>
+  </si>
+  <si>
+    <t>Read four CVs on main (railcom). Reads cv, cv+1, cv+2, cv+3</t>
   </si>
 </sst>
 </file>
@@ -786,11 +792,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C789B9-828D-42BA-9B4D-23D02CCD2FAC}">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,6 +1146,18 @@
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
@@ -1209,70 +1227,61 @@
         <v>28</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" t="s">
-        <v>105</v>
-      </c>
-      <c r="E47" t="s">
-        <v>106</v>
-      </c>
-      <c r="F47" t="s">
-        <v>102</v>
-      </c>
-      <c r="G47" t="s">
-        <v>123</v>
-      </c>
-      <c r="H47" t="s">
-        <v>99</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D48" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" t="s">
         <v>102</v>
       </c>
-      <c r="E48" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" t="s">
-        <v>106</v>
+      <c r="G48" t="s">
+        <v>123</v>
+      </c>
+      <c r="H48" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" t="s">
-        <v>90</v>
-      </c>
-      <c r="F50" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,10 +1292,16 @@
         <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D51" t="s">
         <v>80</v>
+      </c>
+      <c r="E51" t="s">
+        <v>90</v>
+      </c>
+      <c r="F51" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1297,47 +1312,44 @@
         <v>65</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="D52" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" t="s">
-        <v>67</v>
-      </c>
-      <c r="E53" t="s">
-        <v>68</v>
-      </c>
-      <c r="F53" t="s">
-        <v>69</v>
-      </c>
-      <c r="G53" t="s">
-        <v>70</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>65</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>68</v>
+      </c>
+      <c r="F54" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1348,16 +1360,13 @@
         <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D55" t="s">
         <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>76</v>
-      </c>
-      <c r="F55" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1368,10 +1377,16 @@
         <v>65</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D56" t="s">
         <v>80</v>
+      </c>
+      <c r="E56" t="s">
+        <v>76</v>
+      </c>
+      <c r="F56" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1382,7 +1397,10 @@
         <v>65</v>
       </c>
       <c r="C57" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1390,127 +1408,121 @@
         <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" t="s">
-        <v>67</v>
-      </c>
-      <c r="E58" t="s">
-        <v>69</v>
-      </c>
-      <c r="F58" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>67</v>
+      </c>
+      <c r="E59" t="s">
+        <v>69</v>
+      </c>
+      <c r="F59" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64" t="s">
+        <v>100</v>
+      </c>
+      <c r="D64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E64" t="s">
+        <v>98</v>
+      </c>
+      <c r="F64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C65" t="s">
         <v>104</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>102</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>99</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>105</v>
       </c>
-      <c r="G64" t="s">
+      <c r="G65" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C70" t="s">
-        <v>85</v>
-      </c>
-      <c r="D70" t="s">
-        <v>80</v>
-      </c>
-      <c r="E70" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>58</v>
       </c>
@@ -1518,19 +1530,16 @@
         <v>65</v>
       </c>
       <c r="C71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D71" t="s">
         <v>80</v>
       </c>
       <c r="E71" t="s">
-        <v>90</v>
-      </c>
-      <c r="F71" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>58</v>
       </c>
@@ -1538,13 +1547,19 @@
         <v>65</v>
       </c>
       <c r="C72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D72" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>90</v>
+      </c>
+      <c r="F72" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>58</v>
       </c>
@@ -1552,17 +1567,31 @@
         <v>65</v>
       </c>
       <c r="C73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D73" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C74" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B75" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>